<commit_message>
1) Added Title for song text 2) Added border for video and additional info space 3) Icons correctly showing now.
</commit_message>
<xml_diff>
--- a/documentation/plan.xlsx
+++ b/documentation/plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -634,12 +634,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="2" max="2" width="48.7109375" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
@@ -940,7 +941,7 @@
         <v>41350</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>38718</v>
       </c>
@@ -1147,7 +1148,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>76</v>
       </c>

</xml_diff>